<commit_message>
updated the code and files
</commit_message>
<xml_diff>
--- a/test_cases/Automation_Feasibility_Check.xlsx
+++ b/test_cases/Automation_Feasibility_Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ibm-my.sharepoint.com/personal/devanath_kuna_ibm_com/Documents/automation-analyzer/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{47C1D222-1070-4735-93E3-CC7B3491D045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1327A5B-6DE1-4517-BC7F-9E2730902FCD}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{47C1D222-1070-4735-93E3-CC7B3491D045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59BF2845-CA1A-4320-82C5-C8FDDC49C94C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{32056DC8-C916-43B9-9277-06962E97C7E8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>User is logged in only if CAPTCHA is solved correctly. If CAPTCHA is incorrect or skipped, login should be blocked with an appropriate error message</t>
+  </si>
+  <si>
+    <t>Validate login functionality with valid credentials</t>
+  </si>
+  <si>
+    <t>1. Navigate to the login page
+2. Enter valid username and password
+3.Click the login button
+4.Verify successful login message</t>
+  </si>
+  <si>
+    <t>User is redirected to the dashboard with a welcome message</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Verify physical hardware connection and LED status</t>
+  </si>
+  <si>
+    <t>1. Connect the USB device to the machin
+2. Observe the LED indicator on the device
+3.Confirm the LED blinks three times
+4.Disconnect the device and check for safe removal notification</t>
+  </si>
+  <si>
+    <t>LED blinks three times and system shows safe removal</t>
   </si>
   <si>
     <t>1. Navigate to the login page
@@ -469,18 +499,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E5293A-498B-4336-B53E-87A668820EE6}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -506,15 +536,49 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the prompt and UI changes
</commit_message>
<xml_diff>
--- a/test_cases/Automation_Feasibility_Check.xlsx
+++ b/test_cases/Automation_Feasibility_Check.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="43" documentId="8_{47C1D222-1070-4735-93E3-CC7B3491D045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59BF2845-CA1A-4320-82C5-C8FDDC49C94C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{32056DC8-C916-43B9-9277-06962E97C7E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{32056DC8-C916-43B9-9277-06962E97C7E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>